<commit_message>
Added mock data info
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -11,7 +11,7 @@
     <sheet name="Casos de prueba" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">'Casos de prueba'!$A$1:$F$12</definedName>
+    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">'Casos de prueba'!$A$1:$G$12</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t xml:space="preserve">Historia de Usuario</t>
   </si>
@@ -38,6 +38,9 @@
   </si>
   <si>
     <t xml:space="preserve">Pasos seguidos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Datos</t>
   </si>
   <si>
     <t xml:space="preserve">Resultado esperado</t>
@@ -234,21 +237,21 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="38.63"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="105.64"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="84.2"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="96.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="95.59"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="102.06"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="95.59"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="6" style="1" width="102.06"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="95.59"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -270,13 +273,16 @@
       <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="0"/>
+      <c r="G1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="0"/>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:F12"/>
+  <autoFilter ref="A1:G12"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>